<commit_message>
Updated newborn breast feeding report based on new template
</commit_message>
<xml_diff>
--- a/OutputReports/DHIS2 Reports/HTML Reports/Maharashtra/RCH Reports/#12199 Newborn Breastfeeding/29. Newborn Breastfeeding report.xlsx
+++ b/OutputReports/DHIS2 Reports/HTML Reports/Maharashtra/RCH Reports/#12199 Newborn Breastfeeding/29. Newborn Breastfeeding report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45">
   <si>
     <t>State Family Welfare Bureau,Pune</t>
   </si>
@@ -28,7 +28,7 @@
     <t xml:space="preserve">District  </t>
   </si>
   <si>
-    <t xml:space="preserve"> ELA</t>
+    <t>Live Births</t>
   </si>
   <si>
     <t>Public Institutions  Performance</t>
@@ -49,16 +49,10 @@
     <t>Rank</t>
   </si>
   <si>
-    <t>Last year performance upto [February 2017]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diff in absolute (+/-) </t>
-  </si>
-  <si>
-    <t>Annual</t>
-  </si>
-  <si>
-    <t>Prop.</t>
+    <t>During</t>
+  </si>
+  <si>
+    <t>Progressive</t>
   </si>
   <si>
     <t>During Month</t>
@@ -67,13 +61,10 @@
     <t xml:space="preserve">Progressive </t>
   </si>
   <si>
-    <t xml:space="preserve">Annual </t>
-  </si>
-  <si>
-    <t>uC2EhsbN7IV.HllvX50cXC0</t>
-  </si>
-  <si>
-    <t>(C/12)*no. Of months</t>
+    <t>o9GN9y7BcaC.RffjraraKhQ + o9GN9y7BcaC.v7RmjKvAUhD + o9GN9y7BcaC.dWxKPk3OY7I + o9GN9y7BcaC.rZiPexRACnz</t>
+  </si>
+  <si>
+    <t>C column's cumulative data (upto that month in financial year)</t>
   </si>
   <si>
     <t>tSGWouC1jnJ.ZnztZgggxd6 +QbdPC5pcr7M.v7RmjKvAUhD + QbdPC5pcr7M.RffjraraKhQ</t>
@@ -94,7 +85,7 @@
     <t>F+H</t>
   </si>
   <si>
-    <t>(J/C)*100</t>
+    <t>(I/C)*100</t>
   </si>
   <si>
     <t>(J/D)*100</t>
@@ -105,12 +96,6 @@
   </si>
   <si>
     <t>In the order of marks (M); highest=1</t>
-  </si>
-  <si>
-    <t>J in last financial year</t>
-  </si>
-  <si>
-    <t>J-O</t>
   </si>
   <si>
     <t>1. Use following groups for District Total fields:</t>
@@ -173,9 +158,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -231,6 +216,112 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -239,63 +330,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -309,67 +353,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -390,13 +375,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFCCFF99"/>
         <bgColor rgb="FFCCFF99"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,7 +417,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,169 +567,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -672,11 +657,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -698,10 +689,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -717,16 +706,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -755,17 +744,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -774,148 +759,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -944,29 +929,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1288,10 +1273,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1304,10 +1289,9 @@
     <col min="8" max="8" width="23.5714285714286" customWidth="1"/>
     <col min="13" max="13" width="25.5714285714286" customWidth="1"/>
     <col min="14" max="14" width="13.8571428571429" customWidth="1"/>
-    <col min="15" max="15" width="45.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" spans="1:16">
+    <row r="1" ht="17.25" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1324,10 +1308,8 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="7"/>
-    </row>
-    <row r="2" ht="17.25" spans="1:16">
+    </row>
+    <row r="2" ht="17.25" spans="1:14">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1344,10 +1326,8 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="16"/>
-    </row>
-    <row r="3" ht="17.25" spans="1:16">
+    </row>
+    <row r="3" ht="17.25" spans="1:14">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1380,191 +1360,179 @@
       <c r="N3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" ht="34.5" spans="1:16">
+    </row>
+    <row r="4" ht="34.5" spans="1:14">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="G4" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-    </row>
-    <row r="5" ht="90.75" spans="1:16">
+    </row>
+    <row r="5" ht="120" spans="1:14">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="G5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="I5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="J5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="K5" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="L5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="M5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="N5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="11" t="s">
+    </row>
+    <row r="7" ht="22.5" spans="5:7">
+      <c r="E7" s="13"/>
+      <c r="F7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="18" t="s">
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="6:6">
+      <c r="F8" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="18" t="s">
+    </row>
+    <row r="9" spans="6:6">
+      <c r="F9" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="18" t="s">
+    </row>
+    <row r="10" spans="6:6">
+      <c r="F10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="18" t="s">
+    </row>
+    <row r="11" spans="6:6">
+      <c r="F11" s="16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" ht="22.5" spans="6:6">
-      <c r="F7" s="14" t="s">
+    <row r="12" spans="6:6">
+      <c r="F12" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="6:6">
-      <c r="F8" s="15" t="s">
+    <row r="13" spans="6:6">
+      <c r="F13" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="6:6">
-      <c r="F9" s="15" t="s">
+    <row r="14" spans="6:6">
+      <c r="F14" s="16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="6:6">
-      <c r="F10" s="15" t="s">
+    <row r="15" spans="6:6">
+      <c r="F15" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="6:6">
-      <c r="F11" s="15" t="s">
+    <row r="16" spans="6:6">
+      <c r="F16" s="16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="6:6">
-      <c r="F12" s="15" t="s">
+    <row r="17" spans="6:6">
+      <c r="F17" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="6:6">
-      <c r="F13" s="15" t="s">
+    <row r="18" spans="6:6">
+      <c r="F18" s="16" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="6:6">
-      <c r="F14" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="6:6">
-      <c r="F15" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="6:6">
-      <c r="F16" s="15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6">
-      <c r="F17" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6">
-      <c r="F18" s="15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="20" ht="22.5" spans="6:6">
       <c r="F20" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="6:6">
+      <c r="F21" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6">
+      <c r="F22" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6">
+      <c r="F23" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6">
+      <c r="F24" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="6:6">
+      <c r="F25" s="16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="6:6">
-      <c r="F21" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="6:6">
-      <c r="F22" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="6:6">
-      <c r="F23" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="6:6">
-      <c r="F24" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="6:6">
-      <c r="F25" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:P2"/>
+  <mergeCells count="11">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:N2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
@@ -1574,8 +1542,6 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>